<commit_message>
All Data with plot
</commit_message>
<xml_diff>
--- a/Simulated Caregiving - Easy v Demanding - ALL.xlsx
+++ b/Simulated Caregiving - Easy v Demanding - ALL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://missionautismclinics2020-my.sharepoint.com/personal/kglodowski_missionautismclinics_com/Documents/Desktop/Data Science stuff/easy_demanding_caregiving/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="236" documentId="11_E03FE4BD96511D34FF43FAF239B55CF319CBBFC6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8908C52-874F-4092-8E61-035E1B44926D}"/>
+  <xr:revisionPtr revIDLastSave="441" documentId="11_E03FE4BD96511D34FF43FAF239B55CF319CBBFC6" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C2D6C4D3-770A-4632-8F57-8048A1138C5C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="12" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="12" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SP2018-1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1400" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1449" uniqueCount="11">
   <si>
     <t>PreferredItems</t>
   </si>
@@ -90,25 +90,30 @@
   <si>
     <t>One</t>
   </si>
-  <si>
-    <t>% of Intervals with Care_EasyDoll</t>
-  </si>
-  <si>
-    <t>% of Intervals with Care_DemandingDoll</t>
-  </si>
-  <si>
-    <t>Concurrent</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -152,24 +157,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -6021,7 +6028,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:A20"/>
+      <selection activeCell="D1" sqref="D1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10055,7 +10062,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -10063,7 +10070,7 @@
     <col min="1" max="1" width="5.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.33203125" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="4" max="4" width="20.21875" customWidth="1"/>
     <col min="5" max="5" width="20.5546875" customWidth="1"/>
     <col min="6" max="27" width="8.6640625" customWidth="1"/>
   </cols>
@@ -11348,10 +11355,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{648AD3B1-CF10-4443-8C12-3C5197588A7C}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11359,10 +11366,11 @@
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -11375,14 +11383,13 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
@@ -11399,7 +11406,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
@@ -11416,7 +11423,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -11433,7 +11440,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -11446,11 +11453,11 @@
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="F5">
+      <c r="E5">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -11463,11 +11470,11 @@
       <c r="D6">
         <v>5</v>
       </c>
-      <c r="F6">
+      <c r="E6">
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
@@ -11480,11 +11487,11 @@
       <c r="D7">
         <v>6</v>
       </c>
-      <c r="F7">
+      <c r="E7">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
@@ -11501,7 +11508,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
@@ -11518,7 +11525,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
@@ -11535,7 +11542,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
@@ -11548,11 +11555,11 @@
       <c r="D11">
         <v>10</v>
       </c>
-      <c r="F11">
+      <c r="E11">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
@@ -11565,11 +11572,11 @@
       <c r="D12">
         <v>11</v>
       </c>
-      <c r="F12">
+      <c r="E12">
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
@@ -11582,19 +11589,19 @@
       <c r="D13">
         <v>12</v>
       </c>
-      <c r="F13">
+      <c r="E13">
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>13</v>
+      <c r="C14" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="D14">
         <v>13</v>
@@ -11602,87 +11609,157 @@
       <c r="E14">
         <v>15</v>
       </c>
-      <c r="F14">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15">
         <v>13</v>
       </c>
-      <c r="D15">
-        <v>14</v>
-      </c>
       <c r="E15">
-        <v>30</v>
-      </c>
-      <c r="F15">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>13</v>
+      <c r="C16" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="D16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16">
-        <v>10</v>
-      </c>
-      <c r="F16">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>13</v>
+      <c r="C17" s="9" t="s">
+        <v>6</v>
       </c>
       <c r="D17">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E17">
-        <v>15</v>
-      </c>
-      <c r="F17">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C18" s="7" t="s">
-        <v>13</v>
+      <c r="C18" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="D18">
+        <v>15</v>
+      </c>
+      <c r="E18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>15</v>
+      </c>
+      <c r="E19">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20">
+        <v>16</v>
+      </c>
+      <c r="E20">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <v>16</v>
+      </c>
+      <c r="E21">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D22">
         <v>17</v>
       </c>
-      <c r="E18">
-        <v>10</v>
-      </c>
-      <c r="F18">
+      <c r="E22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <v>17</v>
+      </c>
+      <c r="E23">
         <v>50</v>
       </c>
     </row>
@@ -11693,10 +11770,10 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51AFE957-8491-4F7D-8F2E-9123B74A3B7A}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11704,10 +11781,11 @@
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -11720,14 +11798,13 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
@@ -11745,7 +11822,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
@@ -11762,7 +11839,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -11780,7 +11857,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -11798,7 +11875,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -11815,7 +11892,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
@@ -11832,7 +11909,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
@@ -11845,12 +11922,12 @@
       <c r="D8">
         <v>7</v>
       </c>
-      <c r="F8">
+      <c r="E8">
         <f>11/20*100</f>
         <v>55.000000000000007</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
@@ -11863,12 +11940,12 @@
       <c r="D9">
         <v>8</v>
       </c>
-      <c r="F9">
+      <c r="E9">
         <f>13/20*100</f>
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
@@ -11881,20 +11958,20 @@
       <c r="D10">
         <v>9</v>
       </c>
-      <c r="F10">
+      <c r="E10">
         <f>14/20*100</f>
         <v>70</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>13</v>
+      <c r="C11" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -11902,90 +11979,146 @@
       <c r="E11">
         <v>15</v>
       </c>
-      <c r="F11">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>13</v>
+      <c r="C12" s="8" t="s">
+        <v>6</v>
       </c>
       <c r="D12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E12">
-        <v>20</v>
-      </c>
-      <c r="F12">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>13</v>
+      <c r="C13" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="D13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E13">
-        <f>1/20*100</f>
-        <v>5</v>
-      </c>
-      <c r="F13">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>11</v>
+      </c>
+      <c r="E14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
+      </c>
+      <c r="E15">
+        <f>1/20*100</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>12</v>
+      </c>
+      <c r="E16">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17">
         <v>13</v>
       </c>
-      <c r="D14">
+      <c r="E17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18">
         <v>13</v>
       </c>
-      <c r="E14">
-        <v>10</v>
-      </c>
-      <c r="F14">
+      <c r="E18">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11994,10 +12127,10 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D3FBBD-4EA2-4962-8707-93273F4FC545}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12005,10 +12138,11 @@
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -12021,14 +12155,13 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
@@ -12045,7 +12178,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
@@ -12062,7 +12195,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -12079,7 +12212,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -12096,7 +12229,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -12109,12 +12242,12 @@
       <c r="D6">
         <v>5</v>
       </c>
-      <c r="F6">
+      <c r="E6">
         <f>9/20*100</f>
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
@@ -12127,12 +12260,12 @@
       <c r="D7">
         <v>6</v>
       </c>
-      <c r="F7">
+      <c r="E7">
         <f>12/20*100</f>
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
@@ -12145,19 +12278,19 @@
       <c r="D8">
         <v>7</v>
       </c>
-      <c r="F8">
+      <c r="E8">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>13</v>
+      <c r="C9" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="D9">
         <v>8</v>
@@ -12165,72 +12298,99 @@
       <c r="E9">
         <v>15</v>
       </c>
-      <c r="F9">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
         <f>8/20*100</f>
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10">
-        <v>9</v>
-      </c>
-      <c r="E10">
-        <v>20</v>
-      </c>
-      <c r="F10">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="7" t="s">
-        <v>13</v>
+      <c r="C11" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="D11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E11">
-        <v>10</v>
-      </c>
-      <c r="F11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12">
+        <v>9</v>
+      </c>
+      <c r="E12">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="7"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -12244,6 +12404,16 @@
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13676,10 +13846,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28BE7D7A-1CC2-45BF-B140-57D033962F46}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:C13"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13688,10 +13858,10 @@
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -13704,14 +13874,13 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
@@ -13724,12 +13893,12 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="E2">
         <f>14/20*100</f>
         <v>70</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
@@ -13742,11 +13911,11 @@
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="F3">
+      <c r="E3">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -13759,11 +13928,11 @@
       <c r="D4">
         <v>3</v>
       </c>
-      <c r="F4">
+      <c r="E4">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -13776,11 +13945,11 @@
       <c r="D5">
         <v>4</v>
       </c>
-      <c r="F5">
+      <c r="E5">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -13793,12 +13962,12 @@
       <c r="D6">
         <v>5</v>
       </c>
-      <c r="F6">
+      <c r="E6">
         <f>15/20*100</f>
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
@@ -13811,11 +13980,11 @@
       <c r="D7">
         <v>6</v>
       </c>
-      <c r="F7">
+      <c r="E7">
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
@@ -13832,7 +14001,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
@@ -13849,7 +14018,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
@@ -13866,7 +14035,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
@@ -13883,7 +14052,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
@@ -13900,7 +14069,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>10</v>
       </c>
@@ -13913,19 +14082,19 @@
       <c r="D13">
         <v>12</v>
       </c>
-      <c r="F13">
+      <c r="E13">
         <v>60</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>13</v>
+      <c r="C14" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="D14">
         <v>13</v>
@@ -13934,60 +14103,97 @@
         <f>5/20*100</f>
         <v>25</v>
       </c>
-      <c r="F14">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B15" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15">
         <v>13</v>
       </c>
-      <c r="D15">
-        <v>14</v>
-      </c>
       <c r="E15">
-        <v>20</v>
-      </c>
-      <c r="F15">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>13</v>
+      <c r="C16" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="D16">
+        <v>14</v>
+      </c>
+      <c r="E16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>14</v>
+      </c>
+      <c r="E17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18">
         <v>15</v>
       </c>
-      <c r="E16">
-        <v>10</v>
-      </c>
-      <c r="F16">
+      <c r="E18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19">
+        <v>15</v>
+      </c>
+      <c r="E19">
         <f>14/20*100</f>
         <v>70</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13996,10 +14202,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DDCDC6E-D074-49F8-B98C-1B22D8F58407}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14008,10 +14214,11 @@
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
@@ -14024,14 +14231,13 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>10</v>
       </c>
@@ -14044,11 +14250,11 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="E2">
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>10</v>
       </c>
@@ -14061,11 +14267,11 @@
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="F3">
+      <c r="E3">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
         <v>10</v>
       </c>
@@ -14078,11 +14284,11 @@
       <c r="D4">
         <v>3</v>
       </c>
-      <c r="F4">
+      <c r="E4">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
         <v>10</v>
       </c>
@@ -14099,7 +14305,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
         <v>10</v>
       </c>
@@ -14116,7 +14322,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
         <v>10</v>
       </c>
@@ -14133,7 +14339,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
         <v>10</v>
       </c>
@@ -14146,11 +14352,11 @@
       <c r="D8">
         <v>7</v>
       </c>
-      <c r="F8">
+      <c r="E8">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
@@ -14163,11 +14369,11 @@
       <c r="D9">
         <v>8</v>
       </c>
-      <c r="F9">
+      <c r="E9">
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>10</v>
       </c>
@@ -14180,11 +14386,11 @@
       <c r="D10">
         <v>9</v>
       </c>
-      <c r="F10">
+      <c r="E10">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
@@ -14201,7 +14407,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="7" t="s">
         <v>10</v>
       </c>
@@ -14218,15 +14424,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>13</v>
+      <c r="C13" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="D13">
         <v>12</v>
@@ -14234,65 +14440,107 @@
       <c r="E13">
         <v>20</v>
       </c>
-      <c r="F13">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>12</v>
+      </c>
+      <c r="E14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15">
         <v>13</v>
       </c>
-      <c r="D14">
+      <c r="E15">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D16">
         <v>13</v>
       </c>
-      <c r="E14">
-        <v>15</v>
-      </c>
-      <c r="F14">
+      <c r="E16">
         <f>12/20*100</f>
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B15" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D15">
+      <c r="B17" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17">
         <v>14</v>
       </c>
-      <c r="E15">
+      <c r="E17">
         <v>15</v>
       </c>
-      <c r="F15">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>14</v>
+      </c>
+      <c r="E18">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>